<commit_message>
Changes to the project requested by reviewers
Figure labels and titles changed. Technical updates: the functions from the sys_tools.R, lmqc_tools.R and plotting_tools.R scripts are now provided by standalone R packages.
</commit_message>
<xml_diff>
--- a/input data/mod_responses.xlsx
+++ b/input data/mod_responses.xlsx
@@ -52,7 +52,7 @@
     <t xml:space="preserve">binomial</t>
   </si>
   <si>
-    <t xml:space="preserve">CT\nabnormalities @V3</t>
+    <t xml:space="preserve">CT abnormalities\nat 180-day visit</t>
   </si>
   <si>
     <t xml:space="preserve">CT_sev_low</t>
@@ -61,7 +61,7 @@
     <t xml:space="preserve">CT_sev_low_V3</t>
   </si>
   <si>
-    <t xml:space="preserve">CT Severity\nScore @V3 1 – 5</t>
+    <t xml:space="preserve">CT Severity Score 1-5\nat 180-day visit</t>
   </si>
   <si>
     <t xml:space="preserve">CTsevabove5</t>
@@ -70,7 +70,7 @@
     <t xml:space="preserve">CTsevabove5_V3</t>
   </si>
   <si>
-    <t xml:space="preserve">CT Severity\nScore @V3 &gt; 5</t>
+    <t xml:space="preserve">CT Severity Score &gt;5\nat 180-day visit</t>
   </si>
   <si>
     <t xml:space="preserve">sympt_present</t>
@@ -79,7 +79,7 @@
     <t xml:space="preserve">sympt_present_V3</t>
   </si>
   <si>
-    <t xml:space="preserve">Symptoms\npresent @V3</t>
+    <t xml:space="preserve">Symptoms\nat 180-day visit</t>
   </si>
   <si>
     <t xml:space="preserve">lung_function_impaired</t>
@@ -88,7 +88,7 @@
     <t xml:space="preserve">lung_function_impaired_V3</t>
   </si>
   <si>
-    <t xml:space="preserve">Lung function\nimpairment @V3</t>
+    <t xml:space="preserve">Lung function impairment\nat 180-day visit</t>
   </si>
 </sst>
 </file>
@@ -192,10 +192,10 @@
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.61"/>

</xml_diff>